<commit_message>
refactorizaciones en uso de leyendas de color
</commit_message>
<xml_diff>
--- a/src/assets/FESTIVOS.xlsx
+++ b/src/assets/FESTIVOS.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raul.sfernandez\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DESARROLLO\ANGULAR\Babel-holidays\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEB5EBF-0AD2-4F77-A44D-72B65DCD2742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C8E57B-93EB-4769-BF35-59E4922D4730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="25" xr2:uid="{75283843-2193-4F55-866E-37F566EF2A81}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="15" xr2:uid="{75283843-2193-4F55-866E-37F566EF2A81}"/>
   </bookViews>
   <sheets>
     <sheet name="NACIONALES" sheetId="1" r:id="rId1"/>
     <sheet name="AN" sheetId="2" r:id="rId2"/>
     <sheet name="AR" sheetId="4" r:id="rId3"/>
     <sheet name="AS" sheetId="5" r:id="rId4"/>
-    <sheet name="BA" sheetId="6" r:id="rId5"/>
+    <sheet name="IB" sheetId="6" r:id="rId5"/>
     <sheet name="CN-HI" sheetId="7" r:id="rId6"/>
     <sheet name="CN-FU" sheetId="8" r:id="rId7"/>
     <sheet name="CN-GC" sheetId="9" r:id="rId8"/>
@@ -200,7 +200,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd\-mm"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -242,7 +242,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD126649-A0A2-4BB6-80DF-7D0E41893654}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
@@ -1593,7 +1593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD20C5B-8915-48EE-A21A-6F377F22F728}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>